<commit_message>
fetch value from 2 columns and extent report config
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -3,7 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{EDCFCCFF-B703-498F-9D17-9C3E6C748748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\003RXA744\Downloads\SeleniumFramework\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28356998-DE3F-4B97-A169-3B35CECCBA60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,30 +16,32 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>ProductToSearch</t>
   </si>
   <si>
-    <t>Moneycontrol</t>
+    <t>product</t>
   </si>
   <si>
-    <t>Moneycontrol2</t>
+    <t>student</t>
   </si>
   <si>
-    <t>Moneycontrol3</t>
+    <t>Password123</t>
+  </si>
+  <si>
+    <t>student1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -46,6 +53,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -401,35 +414,49 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.21875" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>